<commit_message>
adding scanned docs from rough record
</commit_message>
<xml_diff>
--- a/DOCS/Test Cases.xlsx
+++ b/DOCS/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="48" windowWidth="22980" windowHeight="9024"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="20730" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="62">
   <si>
     <t>S.No</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Should flash appropriate error message</t>
   </si>
   <si>
-    <t>Registration Page</t>
-  </si>
-  <si>
     <t>Enter valid data in all fields</t>
   </si>
   <si>
@@ -81,29 +78,160 @@
     <t>Error message should be flashed.</t>
   </si>
   <si>
-    <t>Add Subject Page</t>
-  </si>
-  <si>
-    <t>Enter valid data in all fileds.</t>
-  </si>
-  <si>
-    <t>Success message should be flashed.</t>
-  </si>
-  <si>
-    <t>Enter a subject code that is already in the data base and try adding the subject.</t>
-  </si>
-  <si>
-    <t>Click the ADD button without entering data in any fileds.</t>
-  </si>
-  <si>
     <t>Automated Question Paper Generator(AQPG) with Blooms Taxonomy Evaluation (V2)</t>
+  </si>
+  <si>
+    <t>Add user Page</t>
+  </si>
+  <si>
+    <t>Add department Page</t>
+  </si>
+  <si>
+    <t>Should flash the "Successfully added" message.</t>
+  </si>
+  <si>
+    <t>Enter a department name that is already in the database.</t>
+  </si>
+  <si>
+    <t>Should flash" department already exist" message.</t>
+  </si>
+  <si>
+    <t>Click add button without entering any fields</t>
+  </si>
+  <si>
+    <t>Add booms keyword Page</t>
+  </si>
+  <si>
+    <t>Try to enter a blooms verb that is already in the database under the same knowledge level.</t>
+  </si>
+  <si>
+    <t>Should flash" blooms verb already exist" message.</t>
+  </si>
+  <si>
+    <t>Add subject Page</t>
+  </si>
+  <si>
+    <t>enter a subject code that is already in the data base.</t>
+  </si>
+  <si>
+    <t>Should flash" subject already exist" message.</t>
+  </si>
+  <si>
+    <t>Map subject Page</t>
+  </si>
+  <si>
+    <t>Try to map a co that is already mapped to a module of the same subject.</t>
+  </si>
+  <si>
+    <t>Should flash" co already mapped" message.</t>
+  </si>
+  <si>
+    <t>Add mark Page</t>
+  </si>
+  <si>
+    <t>enter a non numeric value in the mark field.</t>
+  </si>
+  <si>
+    <t>Should flash" invalid mark" message.</t>
+  </si>
+  <si>
+    <t>Add question Page</t>
+  </si>
+  <si>
+    <t>Try to enter a question that is already in the system for the same subject, module and mark.</t>
+  </si>
+  <si>
+    <t>Similar questions in the database should be displayed under the similar questions heading.</t>
+  </si>
+  <si>
+    <t>Generate qn paper Page</t>
+  </si>
+  <si>
+    <t>Corresponding question paper should be generated in the pdf form in a new tab.</t>
+  </si>
+  <si>
+    <t>Give the total no.of question paper from part A as 0</t>
+  </si>
+  <si>
+    <t>Give the total no.of question paper from part B as 0</t>
+  </si>
+  <si>
+    <t>Qn paper should be generated and flash a message.</t>
+  </si>
+  <si>
+    <t>Give the total no.of question paper from part A as 0 and give correct count in part B.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Give the total no.of question paper from part </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as 0 and give correct count in part A.</t>
+    </r>
+  </si>
+  <si>
+    <t>Click generate button without entering any fields</t>
+  </si>
+  <si>
+    <t>Add newsfeed Page</t>
+  </si>
+  <si>
+    <t>Click post button without entering any fields</t>
+  </si>
+  <si>
+    <t>Add archive Page</t>
+  </si>
+  <si>
+    <t>Try to enter an entry without attaching  a file</t>
+  </si>
+  <si>
+    <t>Load the page</t>
+  </si>
+  <si>
+    <t>Only subjects from the corresponding department of the logged in user should be displayed</t>
+  </si>
+  <si>
+    <t>View subject page</t>
+  </si>
+  <si>
+    <t>view newsfeed page</t>
+  </si>
+  <si>
+    <t>Only newsfeed from the corresponding department of the logged in user should be displayed</t>
+  </si>
+  <si>
+    <t>view archive page</t>
+  </si>
+  <si>
+    <t>Only question papers from the corresponding department of the logged in user should be displayed</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +265,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -505,25 +641,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F18"/>
+  <dimension ref="A2:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="62.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="40.21875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="40.15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>0</v>
@@ -544,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -557,8 +696,14 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -571,8 +716,14 @@
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -585,8 +736,14 @@
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -594,63 +751,87 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -658,46 +839,732 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>18</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>19</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>22</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>24</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>25</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>20</v>
+      <c r="B38" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>26</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>27</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>28</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>29</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>31</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>32</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>33</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>34</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>35</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>36</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>37</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>38</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>39</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -712,7 +1579,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -724,7 +1591,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>